<commit_message>
made CreateReport.py according to Excel file added .gitignore file(any file that inside won't be commited and will be ignored) added to Database.py function to add cities from list
</commit_message>
<xml_diff>
--- a/UserDatabase.xlsx
+++ b/UserDatabase.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -506,7 +506,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CreateReport_Test.py unit test made Register_Test.py unit test made
</commit_message>
<xml_diff>
--- a/UserDatabase.xlsx
+++ b/UserDatabase.xlsx
@@ -1,59 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sman9\Desktop\Git Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12450" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -203,40 +185,109 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="16">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -502,234 +553,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="10" width="14.42578125"/>
+    <col customWidth="1" max="2" min="2" style="10" width="14.28515625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="10" width="22.7109375"/>
+    <col customWidth="1" max="4" min="4" style="10" width="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="14" t="inlineStr">
+        <is>
+          <t>zxcas</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>gred</t>
+        </is>
+      </c>
+      <c r="C2" s="15" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="D2" s="9" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="14" t="inlineStr">
+        <is>
+          <t>MosheShmul</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>sceil567</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
+          <t>moshesh11@ac.sce.ac.il</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="14" t="inlineStr">
+        <is>
+          <t>Amei</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Gishdalah</t>
+        </is>
+      </c>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>gishdalah@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="14" t="inlineStr">
+        <is>
+          <t>Gila</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>iop</t>
+        </is>
+      </c>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>fvasfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>sffs</t>
+        </is>
+      </c>
+      <c r="C6" s="12" t="inlineStr">
+        <is>
+          <t>gjias</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="12" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="14" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="12" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="14" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="12" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="14" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="12" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="12" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="14" t="n"/>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="12" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="14" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="12" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="14" t="n"/>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="12" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="14" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="12" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="14" t="n"/>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="12" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="14" t="n"/>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="12" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="14" t="n"/>
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="12" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="14" t="n"/>
+      <c r="B19" s="1" t="n"/>
+      <c r="C19" s="12" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="14" t="n"/>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="12" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n"/>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="12" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="n"/>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="12" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="n"/>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="12" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="n"/>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="12" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="n"/>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="12" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="n"/>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="12" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="n"/>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="12" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="n"/>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="12" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="n"/>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="12" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="n"/>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="12" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="n"/>
+      <c r="B31" s="1" t="n"/>
+      <c r="C31" s="12" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="n"/>
+      <c r="B32" s="1" t="n"/>
+      <c r="C32" s="12" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="n"/>
+      <c r="B33" s="1" t="n"/>
+      <c r="C33" s="12" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="34" s="10" thickBot="1">
+      <c r="A34" s="6" t="n"/>
+      <c r="B34" s="7" t="n"/>
+      <c r="C34" s="13" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RegisterTkinter.py created still need some touch to avoid registering exsiting username or email
</commit_message>
<xml_diff>
--- a/UserDatabase.xlsx
+++ b/UserDatabase.xlsx
@@ -561,7 +561,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C13" sqref="A7:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -593,7 +593,7 @@
     <row r="2">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>zxcas</t>
+          <t>MaxShap</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -680,53 +680,41 @@
     <row r="7">
       <c r="A7" s="14" t="inlineStr">
         <is>
-          <t>hssdf</t>
+          <t>zMaxShap</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>ny</t>
+          <t>Sfgjk</t>
         </is>
       </c>
       <c r="C7" s="12" t="inlineStr">
         <is>
-          <t>zvfd</t>
+          <t>itsjustmax9@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="14" t="inlineStr">
         <is>
-          <t>uykfkm</t>
+          <t>MaxShap</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>efge</t>
+          <t>Sfgjk</t>
         </is>
       </c>
       <c r="C8" s="12" t="inlineStr">
         <is>
-          <t>uky</t>
+          <t>itsfasfaa</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="inlineStr">
-        <is>
-          <t>hgf</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>jtyj</t>
-        </is>
-      </c>
-      <c r="C9" s="12" t="inlineStr">
-        <is>
-          <t>jhgfjk</t>
-        </is>
-      </c>
+      <c r="A9" s="14" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="12" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="14" t="n"/>

</xml_diff>

<commit_message>
Register - Added Logo on top of the window
</commit_message>
<xml_diff>
--- a/UserDatabase.xlsx
+++ b/UserDatabase.xlsx
@@ -712,14 +712,38 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="inlineStr"/>
-      <c r="B9" s="1" t="inlineStr"/>
-      <c r="C9" s="12" t="inlineStr"/>
+      <c r="A9" s="14" t="inlineStr">
+        <is>
+          <t>zMaxShap</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>asfgfkjlahfs</t>
+        </is>
+      </c>
+      <c r="C9" s="12" t="inlineStr">
+        <is>
+          <t>Sman95@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="14" t="n"/>
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="12" t="n"/>
+      <c r="A10" s="14" t="inlineStr">
+        <is>
+          <t>sfdafg</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>asdasfg</t>
+        </is>
+      </c>
+      <c r="C10" s="12" t="inlineStr">
+        <is>
+          <t>Sman95@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="14" t="n"/>

</xml_diff>

<commit_message>
Added Map to reports(City tab)
</commit_message>
<xml_diff>
--- a/UserDatabase.xlsx
+++ b/UserDatabase.xlsx
@@ -561,7 +561,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="A7:C13"/>
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -680,7 +680,7 @@
     <row r="7">
       <c r="A7" s="14" t="inlineStr">
         <is>
-          <t>zMaxShap</t>
+          <t>safafgas</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -697,113 +697,253 @@
     <row r="8">
       <c r="A8" s="14" t="inlineStr">
         <is>
-          <t>MaxShap</t>
+          <t>zMaxShap</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>Sfgjk</t>
+          <t>asfashjk</t>
         </is>
       </c>
       <c r="C8" s="12" t="inlineStr">
         <is>
-          <t>itsfasfaa</t>
+          <t>Sman95@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="14" t="inlineStr">
         <is>
-          <t>zMaxShap</t>
+          <t>asfda</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>asfgfkjlahfs</t>
+          <t>fasfas</t>
         </is>
       </c>
       <c r="C9" s="12" t="inlineStr">
         <is>
-          <t>Sman95@gmail.com</t>
+          <t>asffa</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="14" t="inlineStr">
         <is>
-          <t>sfdafg</t>
+          <t>fasfa</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>asdasfg</t>
+          <t>asfafa</t>
         </is>
       </c>
       <c r="C10" s="12" t="inlineStr">
         <is>
+          <t>fasf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="14" t="inlineStr">
+        <is>
+          <t>gsdsdg</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>sgdsg</t>
+        </is>
+      </c>
+      <c r="C11" s="12" t="inlineStr">
+        <is>
+          <t>sdgsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="14" t="inlineStr">
+        <is>
+          <t>dfhdgf</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>gfawgfafs</t>
+        </is>
+      </c>
+      <c r="C12" s="12" t="inlineStr">
+        <is>
+          <t>asfasfas</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="14" t="inlineStr">
+        <is>
+          <t>sfafaf</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>asfafs</t>
+        </is>
+      </c>
+      <c r="C13" s="12" t="inlineStr">
+        <is>
           <t>Sman95@gmail.com</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="14" t="n"/>
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="12" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="14" t="n"/>
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="12" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="14" t="n"/>
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="12" t="n"/>
-    </row>
     <row r="14">
-      <c r="A14" s="14" t="n"/>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="12" t="n"/>
+      <c r="A14" s="14" t="inlineStr">
+        <is>
+          <t>asfaf</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>asasf</t>
+        </is>
+      </c>
+      <c r="C14" s="12" t="inlineStr">
+        <is>
+          <t>afs</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="n"/>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="12" t="n"/>
+      <c r="A15" s="14" t="inlineStr">
+        <is>
+          <t>MaxShapira</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>asfnajskflh</t>
+        </is>
+      </c>
+      <c r="C15" s="12" t="inlineStr">
+        <is>
+          <t>Sman95@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="n"/>
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="12" t="n"/>
+      <c r="A16" s="14" t="inlineStr">
+        <is>
+          <t>zMaxShap</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>fjashdfkas</t>
+        </is>
+      </c>
+      <c r="C16" s="12" t="inlineStr">
+        <is>
+          <t>afafgasf</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="14" t="n"/>
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="12" t="n"/>
+      <c r="A17" s="14" t="inlineStr">
+        <is>
+          <t>zMaxShap</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>hasikfl</t>
+        </is>
+      </c>
+      <c r="C17" s="12" t="inlineStr">
+        <is>
+          <t>sdgfjksglfs</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="14" t="n"/>
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="12" t="n"/>
+      <c r="A18" s="14" t="inlineStr">
+        <is>
+          <t>asfjakf</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>dsafjaskfl</t>
+        </is>
+      </c>
+      <c r="C18" s="12" t="inlineStr">
+        <is>
+          <t>Sman95@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="n"/>
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="12" t="n"/>
+      <c r="A19" s="14" t="inlineStr">
+        <is>
+          <t>asfafsjkl</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>aqjisfaj</t>
+        </is>
+      </c>
+      <c r="C19" s="12" t="inlineStr">
+        <is>
+          <t>Sman95@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="n"/>
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="12" t="n"/>
+      <c r="A20" s="14" t="inlineStr">
+        <is>
+          <t>xcvxv</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>cxvxv</t>
+        </is>
+      </c>
+      <c r="C20" s="12" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="12" t="n"/>
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>fasfas</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>fsafasf</t>
+        </is>
+      </c>
+      <c r="C21" s="12" t="inlineStr">
+        <is>
+          <t>asfa</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="n"/>
-      <c r="B22" s="1" t="n"/>
-      <c r="C22" s="12" t="n"/>
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>fsafaf</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>sfasfa</t>
+        </is>
+      </c>
+      <c r="C22" s="12" t="inlineStr">
+        <is>
+          <t>sfafs</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="n"/>

</xml_diff>